<commit_message>
make change in codes improve added the failed and passed excle to send only the participants how haven't received mail
</commit_message>
<xml_diff>
--- a/participants.xlsx
+++ b/participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFC9F6F-3EBA-4014-9AD1-59E6B044B4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21B9086-1040-4E70-A146-53D3A9065EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>tarun</t>
+  </si>
+  <si>
+    <t>2200039159@kluniversity.in</t>
   </si>
 </sst>
 </file>
@@ -158,16 +164,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -478,7 +481,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +505,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="3"/>
@@ -576,7 +579,21 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="2"/>
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>2020</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
@@ -585,6 +602,7 @@
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{6614FC5A-70F1-430B-9396-6FDD81371244}"/>
     <hyperlink ref="C5" r:id="rId2" xr:uid="{5ACA4E15-B228-494B-BE20-46C698BB1AA9}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{C3E9CA02-79BA-46F5-BC09-752BCD265027}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
improved the codes added the requirement.txt file and some details added readme file
</commit_message>
<xml_diff>
--- a/participants.xlsx
+++ b/participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21B9086-1040-4E70-A146-53D3A9065EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5750228D-404F-47A4-9E12-F37F21602A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>2200039159@kluniversity.in</t>
+  </si>
+  <si>
+    <t>Y20</t>
+  </si>
+  <si>
+    <t>Y22</t>
+  </si>
+  <si>
+    <t>Y23</t>
+  </si>
+  <si>
+    <t>Y21</t>
   </si>
 </sst>
 </file>
@@ -481,7 +493,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,8 +535,8 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2">
-        <v>2021</v>
+      <c r="E2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -540,8 +552,8 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>2022</v>
+      <c r="E3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -557,8 +569,8 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4">
-        <v>2023</v>
+      <c r="E4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -574,8 +586,8 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5">
-        <v>2022</v>
+      <c r="E5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -591,8 +603,8 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6">
-        <v>2020</v>
+      <c r="E6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changed the code removed json file
</commit_message>
<xml_diff>
--- a/participants.xlsx
+++ b/participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5750228D-404F-47A4-9E12-F37F21602A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5530D4CB-7D7C-40F5-B169-17EE73E12239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Y21</t>
+  </si>
+  <si>
+    <t>Punendra</t>
+  </si>
+  <si>
+    <t>2200039115@kluniversity.in</t>
   </si>
 </sst>
 </file>
@@ -493,7 +499,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,13 +614,28 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="2"/>
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>2200039115</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{6614FC5A-70F1-430B-9396-6FDD81371244}"/>
     <hyperlink ref="C5" r:id="rId2" xr:uid="{5ACA4E15-B228-494B-BE20-46C698BB1AA9}"/>
     <hyperlink ref="C6" r:id="rId3" xr:uid="{C3E9CA02-79BA-46F5-BC09-752BCD265027}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{D61B6C39-F90A-4328-988A-3D8C53B401AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>